<commit_message>
collection for individual samples
</commit_message>
<xml_diff>
--- a/app/static/project/uploads/PeterTB/metadata.xlsx
+++ b/app/static/project/uploads/PeterTB/metadata.xlsx
@@ -20,9 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
-  <si>
-    <t xml:space="preserve">filename</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
+  <si>
+    <t xml:space="preserve">BAMfilename</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VCFfilename</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FASTQ_r1filename</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FASTQ_r2filename</t>
   </si>
   <si>
     <t xml:space="preserve">sample_id</t>
@@ -121,6 +130,15 @@
     <t xml:space="preserve">SAWC123.bam</t>
   </si>
   <si>
+    <t xml:space="preserve">SAWC123.vcf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAWC123_r1.fastq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAWC123_r2.fastq</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAWC123</t>
   </si>
   <si>
@@ -169,7 +187,19 @@
     <t xml:space="preserve">S</t>
   </si>
   <si>
-    <t xml:space="preserve">123.bam</t>
+    <t xml:space="preserve">TB123.bam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TB123.vcf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TB123_r1.fastq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TB123_r2.fastq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TB123</t>
   </si>
   <si>
     <t xml:space="preserve">IS-0312</t>
@@ -311,37 +341,42 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AI3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="20.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="25.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="21" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="28" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="6.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="33" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="22.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="14.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="25.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="24" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="31" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="36" style="1" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -441,201 +476,228 @@
       <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="AG1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="1" t="n">
         <v>42897</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="K2" s="1" t="n">
         <v>42921</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="1" t="n">
+      <c r="L2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="1" t="n">
         <v>42923</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" s="1" t="n">
+      <c r="N2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" s="1" t="n">
         <v>42926</v>
       </c>
-      <c r="M2" s="1" t="n">
+      <c r="P2" s="1" t="n">
         <v>1354.251</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2" s="1" t="n">
+      <c r="Q2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" s="1" t="n">
         <v>1.83</v>
       </c>
-      <c r="P2" s="1" t="n">
+      <c r="S2" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="R2" s="1" t="n">
+      <c r="T2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" s="1" t="n">
         <v>42979</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T2" s="1" t="n">
+      <c r="V2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W2" s="1" t="n">
         <v>42980</v>
       </c>
-      <c r="U2" s="1" t="n">
+      <c r="X2" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="W2" s="1" t="n">
+      <c r="Y2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z2" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y2" s="1" t="n">
+      <c r="AA2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB2" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="Z2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA2" s="1" t="n">
+      <c r="AC2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD2" s="1" t="n">
         <v>36224</v>
       </c>
-      <c r="AB2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="AE2" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>123</v>
+        <v>55</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="1" t="n">
         <v>42809</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="K3" s="1" t="n">
         <v>42830</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="1" t="n">
+      <c r="L3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="1" t="n">
         <v>42831</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L3" s="1" t="n">
+      <c r="N3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O3" s="1" t="n">
         <v>42926</v>
       </c>
-      <c r="M3" s="1" t="n">
+      <c r="P3" s="1" t="n">
         <v>851.478</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O3" s="1" t="n">
+      <c r="Q3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R3" s="1" t="n">
         <v>2.01</v>
       </c>
-      <c r="P3" s="1" t="n">
+      <c r="S3" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="T3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U3" s="1" t="n">
+        <v>42958</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="W3" s="1" t="n">
+        <v>42959</v>
+      </c>
+      <c r="X3" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z3" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB3" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD3" s="1" t="n">
+        <v>38658</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="R3" s="1" t="n">
-        <v>42958</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="T3" s="1" t="n">
-        <v>42959</v>
-      </c>
-      <c r="U3" s="1" t="n">
-        <v>153</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="W3" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y3" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA3" s="1" t="n">
-        <v>38658</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF3" s="1" t="s">
-        <v>47</v>
+      <c r="AG3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upload project with multiple files per sample
</commit_message>
<xml_diff>
--- a/app/static/project/uploads/PeterTB/metadata.xlsx
+++ b/app/static/project/uploads/PeterTB/metadata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
   <si>
     <t xml:space="preserve">BAMfilename</t>
   </si>
@@ -187,16 +187,10 @@
     <t xml:space="preserve">S</t>
   </si>
   <si>
-    <t xml:space="preserve">TB123.bam</t>
+    <t xml:space="preserve">NULL</t>
   </si>
   <si>
     <t xml:space="preserve">TB123.vcf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TB123_r1.fastq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TB123_r2.fastq</t>
   </si>
   <si>
     <t xml:space="preserve">TB123</t>
@@ -344,7 +338,7 @@
   <dimension ref="A1:AI3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -601,25 +595,25 @@
         <v>56</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>53</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>42</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>42809</v>
@@ -634,7 +628,7 @@
         <v>42831</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O3" s="1" t="n">
         <v>42926</v>
@@ -652,13 +646,13 @@
         <v>20</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="U3" s="1" t="n">
         <v>42958</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="W3" s="1" t="n">
         <v>42959</v>
@@ -667,25 +661,25 @@
         <v>153</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Z3" s="1" t="n">
         <v>29</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="AB3" s="1" t="n">
         <v>23</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AD3" s="1" t="n">
         <v>38658</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AF3" s="1" t="s">
         <v>53</v>

</xml_diff>